<commit_message>
Added PDFBox and implemented PDF functinonality
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +413,9 @@
       <c r="C2" s="4">
         <v>43054</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="4">
+        <v>43055</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -428,7 +430,9 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -458,7 +462,9 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -488,7 +494,9 @@
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into TiTauro"
This reverts commit f651b86be19168fc14447e28d9f07282210f710f, reversing
changes made to 3eef4999450d64299f6ac310c285bbc424b323e4.
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,9 +413,7 @@
       <c r="C2" s="4">
         <v>43054</v>
       </c>
-      <c r="D2" s="4">
-        <v>43055</v>
-      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -430,9 +428,7 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -462,9 +458,7 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="1">
-        <v>3</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -494,9 +488,7 @@
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="1">
-        <v>3</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' into TiTauro""
This reverts commit 05cd9b3335dfc12a1123b2091e4a630027b8b158.
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +413,9 @@
       <c r="C2" s="4">
         <v>43054</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="4">
+        <v>43055</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -428,7 +430,9 @@
       <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -458,7 +462,9 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -488,7 +494,9 @@
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>

</xml_diff>